<commit_message>
Add mail send part
</commit_message>
<xml_diff>
--- a/Main_Controller.xlsx
+++ b/Main_Controller.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDFBDE6-C56C-4183-9C50-4598D2DEFB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1262DA94-E781-4F0E-A871-03BDBE1CA6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainController" sheetId="1" r:id="rId1"/>
     <sheet name="DataSheet" sheetId="9" r:id="rId2"/>
     <sheet name="DB_Connection" sheetId="3" r:id="rId3"/>
-    <sheet name="SSH_CONNECTION" sheetId="4" r:id="rId4"/>
-    <sheet name="JIRA_Connection" sheetId="5" r:id="rId5"/>
-    <sheet name="MAIL_SEND" sheetId="6" r:id="rId6"/>
+    <sheet name="MAIL_SEND" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Sr_No</t>
   </si>
@@ -71,27 +69,6 @@
     <t>TestFlow_Path</t>
   </si>
   <si>
-    <t>DefaultWait_Time</t>
-  </si>
-  <si>
-    <t>MaxResponseTime</t>
-  </si>
-  <si>
-    <t>Availability_alert</t>
-  </si>
-  <si>
-    <t>ResponseTime_alert</t>
-  </si>
-  <si>
-    <t>Multiple_Testcases</t>
-  </si>
-  <si>
-    <t>DB_Connection</t>
-  </si>
-  <si>
-    <t>JIRA_Connection</t>
-  </si>
-  <si>
     <t>AxisMF_Investor_Self_Partial_Unit_Switch.xlsx</t>
   </si>
   <si>
@@ -137,54 +114,9 @@
     <t>1P$$Tmt@uat</t>
   </si>
   <si>
-    <t>Host</t>
-  </si>
-  <si>
-    <t>Port</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>LibertyCar_PolicyBazaar</t>
-  </si>
-  <si>
-    <t>150.242.14.145</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>@pm05ys$2019</t>
-  </si>
-  <si>
-    <t>JIRA_URL</t>
-  </si>
-  <si>
-    <t>JIRA_USERNAME</t>
-  </si>
-  <si>
-    <t>JIRA_PASSWORD</t>
-  </si>
-  <si>
-    <t>JIRA_PROJECTKEY</t>
-  </si>
-  <si>
-    <t>http://192.168.0.104:8080/secure/Dashboard.jspa</t>
-  </si>
-  <si>
-    <t>tapss</t>
-  </si>
-  <si>
-    <t>Apmosys@123</t>
-  </si>
-  <si>
-    <t>TRS100</t>
-  </si>
-  <si>
     <t>HOST</t>
   </si>
   <si>
@@ -209,27 +141,6 @@
     <t>ATTACHMENT_File_Location</t>
   </si>
   <si>
-    <t>tapass@apmosys.in</t>
-  </si>
-  <si>
-    <t>balaram@123</t>
-  </si>
-  <si>
-    <t>lipsa.pradhan@apmosys.in,devendrasing.rajput@apmosys.in</t>
-  </si>
-  <si>
-    <t>Testing New FrameWork</t>
-  </si>
-  <si>
-    <t>Testing The Process.please find the attachment</t>
-  </si>
-  <si>
-    <t>TESTING the framework</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Apmosys2\\Desktop\\Mitra Application TimeLine  Details.xlsx</t>
-  </si>
-  <si>
     <t>ISHINE</t>
   </si>
   <si>
@@ -255,13 +166,37 @@
   </si>
   <si>
     <t>DYNAMIC</t>
+  </si>
+  <si>
+    <t>biswajitkanha11@gmail.com</t>
+  </si>
+  <si>
+    <t>biswajitsahookanha11@gmail.com</t>
+  </si>
+  <si>
+    <t>zfbaqijmtutiejyd</t>
+  </si>
+  <si>
+    <t>kanhabiswajitsahoo11@gmail.com,biswajitkanha316@gmail.com,biswajit.sahoo@apmosys.com</t>
+  </si>
+  <si>
+    <t>Automation Framework Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please find the Automation Test Report Below Table : </t>
+  </si>
+  <si>
+    <t>Please find the attachment for more detailed about report.</t>
+  </si>
+  <si>
+    <t>C:\\Users\\biswa\\eclipse-workspace\\BiswajitFramework\\DYNAMIC_RESULT\\SummaryTable.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -326,6 +261,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -450,7 +391,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -533,6 +474,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -928,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -963,7 +907,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -986,7 +930,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6">
@@ -1000,16 +944,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6">
@@ -1017,22 +961,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.6">
@@ -1131,7 +1075,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1150,27 +1094,13 @@
       <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>19</v>
-      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
     </row>
@@ -1182,55 +1112,25 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>21</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="28">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="29">
-        <v>10</v>
-      </c>
-      <c r="E3" s="29">
-        <v>60</v>
-      </c>
-      <c r="F3" s="29">
-        <v>0</v>
-      </c>
-      <c r="G3" s="29">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>6</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
       <c r="L3" s="27"/>
@@ -1240,10 +1140,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1277,25 +1177,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="31" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1306,19 +1206,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1391,13 +1291,13 @@
     </row>
     <row r="17" spans="4:6">
       <c r="D17" s="27" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1410,252 +1310,111 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426D32CD-7B6C-4E91-A118-3E64442A7EBC}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" customWidth="1"/>
-    <col min="8" max="8" width="43.88671875" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1"/>
-    <col min="10" max="10" width="32.88671875" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="106.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>51</v>
-      </c>
       <c r="D1" s="32" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="K1" s="32" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.6">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>59</v>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{41B875E8-23BE-4DB8-A1FA-B36821D5E452}"/>
+    <hyperlink ref="E2" r:id="rId2" display="balaram@123" xr:uid="{4069F095-E72A-4853-B5EF-79367E435E66}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{79C1DE28-C011-4DDD-B6FF-85C567026535}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change the result file folder name modify new way
</commit_message>
<xml_diff>
--- a/Main_Controller.xlsx
+++ b/Main_Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D47DB2-C1C3-40C6-9C15-A388E8CFF878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94442A04-A0E2-4805-B233-81CE19F91C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainController" sheetId="1" r:id="rId1"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -1278,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426D32CD-7B6C-4E91-A118-3E64442A7EBC}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>